<commit_message>
Definition file change and bug fix
</commit_message>
<xml_diff>
--- a/Deployment/colTranslation.xlsx
+++ b/Deployment/colTranslation.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
   <si>
     <t>Locale</t>
   </si>
@@ -577,9 +577,6 @@
   </si>
   <si>
     <t>RequestClosedSuccess</t>
-  </si>
-  <si>
-    <t>Request closed sucessfully!</t>
   </si>
   <si>
     <t>Title is required</t>
@@ -670,6 +667,12 @@
   </si>
   <si>
     <t>Experts</t>
+  </si>
+  <si>
+    <t>RequestClosedSuccessMsg</t>
+  </si>
+  <si>
+    <t>Request closed successfully!</t>
   </si>
 </sst>
 </file>
@@ -829,9 +832,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="colTranslationadmin" displayName="colTranslationadmin" ref="A1:CC7" totalsRowShown="0">
-  <autoFilter ref="A1:CC7"/>
-  <tableColumns count="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="colTranslationadmin" displayName="colTranslationadmin" ref="A1:CD7" totalsRowShown="0">
+  <autoFilter ref="A1:CD7"/>
+  <tableColumns count="82">
     <tableColumn id="1" name="Locale"/>
     <tableColumn id="2" name="IsSupported"/>
     <tableColumn id="3" name="WelcomeMessage"/>
@@ -912,6 +915,7 @@
     <tableColumn id="78" name="NoSearchResultFound"/>
     <tableColumn id="80" name="ExpertViewGridLabel"/>
     <tableColumn id="81" name="ChannelViewGridLabel"/>
+    <tableColumn id="82" name="RequestClosedSuccessMsg"/>
     <tableColumn id="79" name="updatedby"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1183,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,25 +1414,25 @@
         <v>52</v>
       </c>
       <c r="BB1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BC1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BD1" t="s">
         <v>53</v>
       </c>
       <c r="BE1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BF1" t="s">
         <v>192</v>
       </c>
-      <c r="BF1" t="s">
-        <v>193</v>
-      </c>
       <c r="BG1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BH1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1547,7 +1551,7 @@
         <v>80</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AN2" t="s">
         <v>39</v>
@@ -1592,25 +1596,25 @@
         <v>89</v>
       </c>
       <c r="BB2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BC2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BD2" t="s">
         <v>90</v>
       </c>
       <c r="BE2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BF2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BG2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BH2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1625,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC2"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CB4" sqref="CB4"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
+      <selection activeCell="BY2" sqref="BY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,11 +1701,11 @@
     <col min="69" max="69" width="39.42578125" customWidth="1"/>
     <col min="70" max="70" width="22.28515625" customWidth="1"/>
     <col min="71" max="76" width="47.28515625" customWidth="1"/>
-    <col min="77" max="80" width="30.28515625" customWidth="1"/>
-    <col min="81" max="81" width="22.42578125" customWidth="1"/>
+    <col min="77" max="81" width="30.28515625" customWidth="1"/>
+    <col min="82" max="82" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1934,19 +1938,22 @@
         <v>141</v>
       </c>
       <c r="BZ1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CA1" t="s">
+        <v>202</v>
+      </c>
+      <c r="CB1" t="s">
         <v>203</v>
       </c>
-      <c r="CB1" t="s">
-        <v>204</v>
-      </c>
       <c r="CC1" t="s">
-        <v>202</v>
+        <v>205</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:81" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:82" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1993,7 +2000,7 @@
         <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
@@ -2080,16 +2087,16 @@
         <v>39</v>
       </c>
       <c r="AS2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AT2" t="s">
         <v>160</v>
       </c>
       <c r="AU2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AV2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AW2" t="s">
         <v>122</v>
@@ -2131,7 +2138,7 @@
         <v>165</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="BK2" s="2" t="s">
         <v>132</v>
@@ -2173,22 +2180,25 @@
         <v>181</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="BY2" t="s">
         <v>179</v>
       </c>
       <c r="BZ2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CA2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="CB2" t="s">
         <v>106</v>
       </c>
       <c r="CC2" t="s">
-        <v>201</v>
+        <v>206</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded packages to fix localization issues
</commit_message>
<xml_diff>
--- a/Deployment/colTranslation.xlsx
+++ b/Deployment/colTranslation.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="206">
   <si>
     <t>Locale</t>
   </si>
@@ -244,9 +244,6 @@
     <t>Status:</t>
   </si>
   <si>
-    <t>ConnectwithExpertsScreenDirect</t>
-  </si>
-  <si>
     <t>Request details</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Join meeting</t>
   </si>
   <si>
-    <t>We've set up your meeting! Join now. A expert will soon assist you.</t>
-  </si>
-  <si>
     <t>Filter by keyword</t>
   </si>
   <si>
@@ -290,12 +284,6 @@
   </si>
   <si>
     <t>Talk to an expert now</t>
-  </si>
-  <si>
-    <t>Please wait... meeting link is not ready","Meeting link is ready.</t>
-  </si>
-  <si>
-    <t>Meeting Scheduled, please click on join.</t>
   </si>
   <si>
     <t>No query available</t>
@@ -531,9 +519,6 @@
     <t>Type content</t>
   </si>
   <si>
-    <t>Are you sure you want to delete category?</t>
-  </si>
-  <si>
     <t>Are you sure you want to delete this topic?</t>
   </si>
   <si>
@@ -615,10 +600,34 @@
     <t>JoinNow</t>
   </si>
   <si>
-    <t>A expert will soon assist you</t>
-  </si>
-  <si>
     <t>ExpertAssistanceMessage</t>
+  </si>
+  <si>
+    <t>Requested by:</t>
+  </si>
+  <si>
+    <t>Max 3 experts can be selected</t>
+  </si>
+  <si>
+    <t>updatedby</t>
+  </si>
+  <si>
+    <t>ExpertViewGridLabel</t>
+  </si>
+  <si>
+    <t>ChannelViewGridLabel</t>
+  </si>
+  <si>
+    <t>Experts</t>
+  </si>
+  <si>
+    <t>RequestClosedSuccessMsg</t>
+  </si>
+  <si>
+    <t>Request closed successfully!</t>
+  </si>
+  <si>
+    <t>An expert will soon assist you</t>
   </si>
   <si>
     <r>
@@ -644,35 +653,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> button apppears.</t>
+      <t xml:space="preserve"> button appears.</t>
     </r>
   </si>
   <si>
-    <t>Requested by:</t>
-  </si>
-  <si>
-    <t>Max 3 experts can be selected</t>
-  </si>
-  <si>
-    <t>updated by</t>
-  </si>
-  <si>
-    <t>updatedby</t>
-  </si>
-  <si>
-    <t>ExpertViewGridLabel</t>
-  </si>
-  <si>
-    <t>ChannelViewGridLabel</t>
-  </si>
-  <si>
-    <t>Experts</t>
-  </si>
-  <si>
-    <t>RequestClosedSuccessMsg</t>
-  </si>
-  <si>
-    <t>Request closed successfully!</t>
+    <t>Connect with experts screen direct</t>
+  </si>
+  <si>
+    <t>We've set up your meeting! Join now. An expert will soon assist you.</t>
+  </si>
+  <si>
+    <t>Meeting scheduled, please click on join.</t>
+  </si>
+  <si>
+    <t>Please wait... meeting link is not ready.</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete this category?</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1208,15 @@
     <col min="16" max="16" width="43.7109375" customWidth="1"/>
     <col min="17" max="17" width="29" customWidth="1"/>
     <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="20" max="20" width="50.5703125" customWidth="1"/>
     <col min="21" max="21" width="34.7109375" customWidth="1"/>
     <col min="22" max="22" width="35.7109375" customWidth="1"/>
     <col min="23" max="23" width="39.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="33" hidden="1" customWidth="1"/>
+    <col min="24" max="25" width="18.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" customWidth="1"/>
+    <col min="27" max="27" width="36.140625" customWidth="1"/>
+    <col min="28" max="28" width="32.28515625" customWidth="1"/>
+    <col min="29" max="29" width="21.7109375" customWidth="1"/>
     <col min="30" max="30" width="39.7109375" customWidth="1"/>
     <col min="31" max="31" width="41" customWidth="1"/>
     <col min="32" max="32" width="68" customWidth="1"/>
@@ -1233,21 +1230,20 @@
     <col min="41" max="41" width="92.28515625" customWidth="1"/>
     <col min="42" max="42" width="67.28515625" customWidth="1"/>
     <col min="43" max="43" width="33.28515625" customWidth="1"/>
-    <col min="44" max="44" width="31" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="23.42578125" customWidth="1"/>
+    <col min="44" max="44" width="14" customWidth="1"/>
+    <col min="45" max="46" width="23.42578125" customWidth="1"/>
     <col min="47" max="47" width="5" customWidth="1"/>
-    <col min="48" max="48" width="23.42578125" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="19.28515625" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="19" customWidth="1"/>
+    <col min="49" max="49" width="13.85546875" customWidth="1"/>
     <col min="50" max="50" width="26.28515625" customWidth="1"/>
     <col min="51" max="51" width="10.42578125" customWidth="1"/>
-    <col min="52" max="52" width="21.7109375" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="33.85546875" customWidth="1"/>
     <col min="53" max="53" width="76.7109375" customWidth="1"/>
     <col min="54" max="54" width="66.42578125" customWidth="1"/>
     <col min="55" max="55" width="26" customWidth="1"/>
     <col min="56" max="56" width="21.28515625" customWidth="1"/>
     <col min="57" max="57" width="19.7109375" customWidth="1"/>
-    <col min="58" max="58" width="36.85546875" customWidth="1"/>
+    <col min="58" max="58" width="62.5703125" customWidth="1"/>
     <col min="59" max="59" width="40.7109375" customWidth="1"/>
     <col min="60" max="60" width="37.5703125" customWidth="1"/>
     <col min="61" max="61" width="36.42578125" customWidth="1"/>
@@ -1414,25 +1410,25 @@
         <v>52</v>
       </c>
       <c r="BB1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="BC1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="BD1" t="s">
         <v>53</v>
       </c>
       <c r="BE1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="BF1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="BG1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="BH1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1511,7 @@
         <v>25</v>
       </c>
       <c r="AA2" t="s">
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="AB2" t="s">
         <v>26</v>
@@ -1524,61 +1520,61 @@
         <v>63</v>
       </c>
       <c r="AD2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE2" t="s">
         <v>73</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>74</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>75</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>77</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>78</v>
       </c>
       <c r="AJ2" t="s">
         <v>62</v>
       </c>
       <c r="AK2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AN2" t="s">
         <v>39</v>
       </c>
       <c r="AO2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AP2" t="s">
         <v>15</v>
       </c>
       <c r="AQ2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS2" t="s">
         <v>82</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="AW2" t="s">
         <v>48</v>
@@ -1590,31 +1586,31 @@
         <v>50</v>
       </c>
       <c r="AZ2" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="BA2" t="s">
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="BB2" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG2" t="s">
         <v>188</v>
       </c>
-      <c r="BC2" t="s">
-        <v>186</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>190</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>185</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>193</v>
-      </c>
       <c r="BH2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1631,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
-      <selection activeCell="BY2" sqref="BY2"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CD5" sqref="CD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,11 +1654,11 @@
     <col min="20" max="20" width="23.28515625" customWidth="1"/>
     <col min="21" max="21" width="31.7109375" customWidth="1"/>
     <col min="22" max="23" width="37.7109375" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" customWidth="1"/>
     <col min="25" max="25" width="26" customWidth="1"/>
     <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="25.7109375" customWidth="1"/>
+    <col min="27" max="27" width="0.42578125" customWidth="1"/>
+    <col min="28" max="28" width="42" customWidth="1"/>
     <col min="29" max="29" width="40.5703125" customWidth="1"/>
     <col min="30" max="30" width="19.7109375" customWidth="1"/>
     <col min="31" max="36" width="8.7109375" hidden="1" customWidth="1"/>
@@ -1722,25 +1718,25 @@
         <v>46</v>
       </c>
       <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" t="s">
-        <v>95</v>
       </c>
       <c r="K1" t="s">
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M1" t="s">
         <v>31</v>
@@ -1752,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Q1" t="s">
         <v>21</v>
@@ -1761,64 +1757,64 @@
         <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="T1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="U1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="V1" t="s">
         <v>24</v>
       </c>
       <c r="W1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="X1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Y1" t="s">
         <v>32</v>
       </c>
       <c r="Z1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" t="s">
         <v>103</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>104</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>105</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>106</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>110</v>
       </c>
       <c r="AH1" t="s">
         <v>19</v>
       </c>
       <c r="AI1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AJ1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AK1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AL1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AM1" t="s">
         <v>39</v>
@@ -1830,52 +1826,52 @@
         <v>40</v>
       </c>
       <c r="AP1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" t="s">
         <v>115</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AU1" t="s">
         <v>116</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AV1" t="s">
         <v>117</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AW1" t="s">
         <v>118</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AX1" t="s">
         <v>119</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>120</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>121</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>122</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>123</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>124</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>127</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>128</v>
       </c>
       <c r="BD1" t="s">
         <v>49</v>
       </c>
       <c r="BE1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="BF1" s="2" t="s">
         <v>45</v>
@@ -1887,70 +1883,70 @@
         <v>5</v>
       </c>
       <c r="BI1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BM1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BO1" t="s">
         <v>132</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BP1" t="s">
         <v>133</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BQ1" t="s">
         <v>134</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BR1" t="s">
         <v>135</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BS1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BT1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY1" t="s">
         <v>137</v>
       </c>
-      <c r="BQ1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BS1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BZ1" t="s">
         <v>182</v>
       </c>
-      <c r="BY1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>187</v>
-      </c>
       <c r="CA1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="CB1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="CC1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="CD1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:82" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1961,46 +1957,46 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>144</v>
       </c>
-      <c r="G2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" t="s">
-        <v>148</v>
-      </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
         <v>75</v>
-      </c>
-      <c r="N2" t="s">
-        <v>76</v>
       </c>
       <c r="O2" t="s">
         <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
@@ -2009,64 +2005,64 @@
         <v>71</v>
       </c>
       <c r="S2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V2" t="s">
         <v>24</v>
       </c>
       <c r="W2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="X2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Y2" t="s">
         <v>15</v>
       </c>
       <c r="Z2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" t="s">
         <v>153</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>157</v>
-      </c>
       <c r="AG2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AH2" t="s">
         <v>68</v>
       </c>
       <c r="AI2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AJ2" t="s">
         <v>63</v>
       </c>
       <c r="AK2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AL2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AM2" t="s">
         <v>39</v>
@@ -2075,130 +2071,130 @@
         <v>48</v>
       </c>
       <c r="AO2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AP2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AQ2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="AR2" t="s">
         <v>39</v>
       </c>
       <c r="AS2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AT2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AU2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AV2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AW2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AX2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AY2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AZ2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="BA2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="BB2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="BC2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="BD2" t="s">
         <v>49</v>
       </c>
       <c r="BE2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="BG2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BH2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="BO2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BT2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="BP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>168</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>139</v>
-      </c>
-      <c r="BS2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="BT2" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="BU2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY2" t="s">
         <v>174</v>
       </c>
-      <c r="BV2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BW2" s="3" t="s">
+      <c r="BZ2" t="s">
         <v>181</v>
       </c>
-      <c r="BX2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>179</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>186</v>
-      </c>
       <c r="CA2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="CB2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="CC2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="CD2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded packages to fix localization issues (#3)
</commit_message>
<xml_diff>
--- a/Deployment/colTranslation.xlsx
+++ b/Deployment/colTranslation.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="206">
   <si>
     <t>Locale</t>
   </si>
@@ -244,9 +244,6 @@
     <t>Status:</t>
   </si>
   <si>
-    <t>ConnectwithExpertsScreenDirect</t>
-  </si>
-  <si>
     <t>Request details</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Join meeting</t>
   </si>
   <si>
-    <t>We've set up your meeting! Join now. A expert will soon assist you.</t>
-  </si>
-  <si>
     <t>Filter by keyword</t>
   </si>
   <si>
@@ -290,12 +284,6 @@
   </si>
   <si>
     <t>Talk to an expert now</t>
-  </si>
-  <si>
-    <t>Please wait... meeting link is not ready","Meeting link is ready.</t>
-  </si>
-  <si>
-    <t>Meeting Scheduled, please click on join.</t>
   </si>
   <si>
     <t>No query available</t>
@@ -531,9 +519,6 @@
     <t>Type content</t>
   </si>
   <si>
-    <t>Are you sure you want to delete category?</t>
-  </si>
-  <si>
     <t>Are you sure you want to delete this topic?</t>
   </si>
   <si>
@@ -615,10 +600,34 @@
     <t>JoinNow</t>
   </si>
   <si>
-    <t>A expert will soon assist you</t>
-  </si>
-  <si>
     <t>ExpertAssistanceMessage</t>
+  </si>
+  <si>
+    <t>Requested by:</t>
+  </si>
+  <si>
+    <t>Max 3 experts can be selected</t>
+  </si>
+  <si>
+    <t>updatedby</t>
+  </si>
+  <si>
+    <t>ExpertViewGridLabel</t>
+  </si>
+  <si>
+    <t>ChannelViewGridLabel</t>
+  </si>
+  <si>
+    <t>Experts</t>
+  </si>
+  <si>
+    <t>RequestClosedSuccessMsg</t>
+  </si>
+  <si>
+    <t>Request closed successfully!</t>
+  </si>
+  <si>
+    <t>An expert will soon assist you</t>
   </si>
   <si>
     <r>
@@ -644,35 +653,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> button apppears.</t>
+      <t xml:space="preserve"> button appears.</t>
     </r>
   </si>
   <si>
-    <t>Requested by:</t>
-  </si>
-  <si>
-    <t>Max 3 experts can be selected</t>
-  </si>
-  <si>
-    <t>updated by</t>
-  </si>
-  <si>
-    <t>updatedby</t>
-  </si>
-  <si>
-    <t>ExpertViewGridLabel</t>
-  </si>
-  <si>
-    <t>ChannelViewGridLabel</t>
-  </si>
-  <si>
-    <t>Experts</t>
-  </si>
-  <si>
-    <t>RequestClosedSuccessMsg</t>
-  </si>
-  <si>
-    <t>Request closed successfully!</t>
+    <t>Connect with experts screen direct</t>
+  </si>
+  <si>
+    <t>We've set up your meeting! Join now. An expert will soon assist you.</t>
+  </si>
+  <si>
+    <t>Meeting scheduled, please click on join.</t>
+  </si>
+  <si>
+    <t>Please wait... meeting link is not ready.</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete this category?</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1208,15 @@
     <col min="16" max="16" width="43.7109375" customWidth="1"/>
     <col min="17" max="17" width="29" customWidth="1"/>
     <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="20" max="20" width="50.5703125" customWidth="1"/>
     <col min="21" max="21" width="34.7109375" customWidth="1"/>
     <col min="22" max="22" width="35.7109375" customWidth="1"/>
     <col min="23" max="23" width="39.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="33" hidden="1" customWidth="1"/>
+    <col min="24" max="25" width="18.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" customWidth="1"/>
+    <col min="27" max="27" width="36.140625" customWidth="1"/>
+    <col min="28" max="28" width="32.28515625" customWidth="1"/>
+    <col min="29" max="29" width="21.7109375" customWidth="1"/>
     <col min="30" max="30" width="39.7109375" customWidth="1"/>
     <col min="31" max="31" width="41" customWidth="1"/>
     <col min="32" max="32" width="68" customWidth="1"/>
@@ -1233,21 +1230,20 @@
     <col min="41" max="41" width="92.28515625" customWidth="1"/>
     <col min="42" max="42" width="67.28515625" customWidth="1"/>
     <col min="43" max="43" width="33.28515625" customWidth="1"/>
-    <col min="44" max="44" width="31" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="23.42578125" customWidth="1"/>
+    <col min="44" max="44" width="14" customWidth="1"/>
+    <col min="45" max="46" width="23.42578125" customWidth="1"/>
     <col min="47" max="47" width="5" customWidth="1"/>
-    <col min="48" max="48" width="23.42578125" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="19.28515625" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="19" customWidth="1"/>
+    <col min="49" max="49" width="13.85546875" customWidth="1"/>
     <col min="50" max="50" width="26.28515625" customWidth="1"/>
     <col min="51" max="51" width="10.42578125" customWidth="1"/>
-    <col min="52" max="52" width="21.7109375" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="33.85546875" customWidth="1"/>
     <col min="53" max="53" width="76.7109375" customWidth="1"/>
     <col min="54" max="54" width="66.42578125" customWidth="1"/>
     <col min="55" max="55" width="26" customWidth="1"/>
     <col min="56" max="56" width="21.28515625" customWidth="1"/>
     <col min="57" max="57" width="19.7109375" customWidth="1"/>
-    <col min="58" max="58" width="36.85546875" customWidth="1"/>
+    <col min="58" max="58" width="62.5703125" customWidth="1"/>
     <col min="59" max="59" width="40.7109375" customWidth="1"/>
     <col min="60" max="60" width="37.5703125" customWidth="1"/>
     <col min="61" max="61" width="36.42578125" customWidth="1"/>
@@ -1414,25 +1410,25 @@
         <v>52</v>
       </c>
       <c r="BB1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="BC1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="BD1" t="s">
         <v>53</v>
       </c>
       <c r="BE1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="BF1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="BG1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="BH1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1511,7 @@
         <v>25</v>
       </c>
       <c r="AA2" t="s">
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="AB2" t="s">
         <v>26</v>
@@ -1524,61 +1520,61 @@
         <v>63</v>
       </c>
       <c r="AD2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE2" t="s">
         <v>73</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>74</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>75</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>77</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>78</v>
       </c>
       <c r="AJ2" t="s">
         <v>62</v>
       </c>
       <c r="AK2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AN2" t="s">
         <v>39</v>
       </c>
       <c r="AO2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AP2" t="s">
         <v>15</v>
       </c>
       <c r="AQ2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS2" t="s">
         <v>82</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="AW2" t="s">
         <v>48</v>
@@ -1590,31 +1586,31 @@
         <v>50</v>
       </c>
       <c r="AZ2" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="BA2" t="s">
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="BB2" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG2" t="s">
         <v>188</v>
       </c>
-      <c r="BC2" t="s">
-        <v>186</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>190</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>185</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>193</v>
-      </c>
       <c r="BH2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1631,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
-      <selection activeCell="BY2" sqref="BY2"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CD5" sqref="CD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,11 +1654,11 @@
     <col min="20" max="20" width="23.28515625" customWidth="1"/>
     <col min="21" max="21" width="31.7109375" customWidth="1"/>
     <col min="22" max="23" width="37.7109375" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" customWidth="1"/>
     <col min="25" max="25" width="26" customWidth="1"/>
     <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="25.7109375" customWidth="1"/>
+    <col min="27" max="27" width="0.42578125" customWidth="1"/>
+    <col min="28" max="28" width="42" customWidth="1"/>
     <col min="29" max="29" width="40.5703125" customWidth="1"/>
     <col min="30" max="30" width="19.7109375" customWidth="1"/>
     <col min="31" max="36" width="8.7109375" hidden="1" customWidth="1"/>
@@ -1722,25 +1718,25 @@
         <v>46</v>
       </c>
       <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" t="s">
-        <v>95</v>
       </c>
       <c r="K1" t="s">
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M1" t="s">
         <v>31</v>
@@ -1752,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Q1" t="s">
         <v>21</v>
@@ -1761,64 +1757,64 @@
         <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="T1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="U1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="V1" t="s">
         <v>24</v>
       </c>
       <c r="W1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="X1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Y1" t="s">
         <v>32</v>
       </c>
       <c r="Z1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" t="s">
         <v>103</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>104</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>105</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>106</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>110</v>
       </c>
       <c r="AH1" t="s">
         <v>19</v>
       </c>
       <c r="AI1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AJ1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AK1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AL1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AM1" t="s">
         <v>39</v>
@@ -1830,52 +1826,52 @@
         <v>40</v>
       </c>
       <c r="AP1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" t="s">
         <v>115</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AU1" t="s">
         <v>116</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AV1" t="s">
         <v>117</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AW1" t="s">
         <v>118</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AX1" t="s">
         <v>119</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>120</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>121</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>122</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>123</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>124</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>127</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>128</v>
       </c>
       <c r="BD1" t="s">
         <v>49</v>
       </c>
       <c r="BE1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="BF1" s="2" t="s">
         <v>45</v>
@@ -1887,70 +1883,70 @@
         <v>5</v>
       </c>
       <c r="BI1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BM1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BO1" t="s">
         <v>132</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BP1" t="s">
         <v>133</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BQ1" t="s">
         <v>134</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BR1" t="s">
         <v>135</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BS1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BT1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY1" t="s">
         <v>137</v>
       </c>
-      <c r="BQ1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BS1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BZ1" t="s">
         <v>182</v>
       </c>
-      <c r="BY1" t="s">
-        <v>141</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>187</v>
-      </c>
       <c r="CA1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="CB1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="CC1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="CD1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:82" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1961,46 +1957,46 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>144</v>
       </c>
-      <c r="G2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" t="s">
-        <v>148</v>
-      </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
         <v>75</v>
-      </c>
-      <c r="N2" t="s">
-        <v>76</v>
       </c>
       <c r="O2" t="s">
         <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
@@ -2009,64 +2005,64 @@
         <v>71</v>
       </c>
       <c r="S2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V2" t="s">
         <v>24</v>
       </c>
       <c r="W2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="X2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Y2" t="s">
         <v>15</v>
       </c>
       <c r="Z2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" t="s">
         <v>153</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>157</v>
-      </c>
       <c r="AG2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AH2" t="s">
         <v>68</v>
       </c>
       <c r="AI2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AJ2" t="s">
         <v>63</v>
       </c>
       <c r="AK2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AL2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AM2" t="s">
         <v>39</v>
@@ -2075,130 +2071,130 @@
         <v>48</v>
       </c>
       <c r="AO2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AP2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="AQ2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="AR2" t="s">
         <v>39</v>
       </c>
       <c r="AS2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AT2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AU2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AV2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AW2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AX2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AY2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AZ2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="BA2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="BB2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="BC2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="BD2" t="s">
         <v>49</v>
       </c>
       <c r="BE2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="BG2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BH2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="BO2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BT2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="BP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>168</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>139</v>
-      </c>
-      <c r="BS2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="BT2" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="BU2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY2" t="s">
         <v>174</v>
       </c>
-      <c r="BV2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BW2" s="3" t="s">
+      <c r="BZ2" t="s">
         <v>181</v>
       </c>
-      <c r="BX2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>179</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>186</v>
-      </c>
       <c r="CA2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="CB2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="CC2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="CD2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>